<commit_message>
Various updates of IFR flights
</commit_message>
<xml_diff>
--- a/data/ifr_flights.xlsx
+++ b/data/ifr_flights.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\oburdash\dev\repos\standard_inputs\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cyven\dev\repos\standard_inputs\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E513A4F-B465-49BE-816E-198C8AD81BCC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2EFD8C3-60AC-4051-A168-929F75B3B8C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="18240" tabRatio="541" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" tabRatio="541" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ifrflight" sheetId="22" r:id="rId1"/>
@@ -525,19 +525,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FCE50129-AC0B-4378-9BC4-EE98C90A7689}">
-  <dimension ref="A1:I29"/>
+  <dimension ref="A1:I14"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="87" workbookViewId="0">
-      <selection activeCell="P26" sqref="P26"/>
+      <selection activeCell="H2" sqref="H2:H14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="8" width="12.85546875" customWidth="1"/>
+    <col min="1" max="8" width="12.88671875" customWidth="1"/>
     <col min="9" max="9" width="23" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>12</v>
       </c>
@@ -563,7 +563,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -586,11 +586,12 @@
         <v>787503</v>
       </c>
       <c r="H2" s="1">
-        <v>-0.63768518977070565</v>
+        <f>F2/G2</f>
+        <v>0.36231481022929435</v>
       </c>
       <c r="I2" s="2"/>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -613,11 +614,12 @@
         <v>737763</v>
       </c>
       <c r="H3" s="1">
-        <v>-0.66125435946232058</v>
+        <f>F3/G3</f>
+        <v>0.33874564053767947</v>
       </c>
       <c r="I3" s="2"/>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -640,11 +642,12 @@
         <v>846442</v>
       </c>
       <c r="H4" s="1">
-        <v>-0.63720963751798698</v>
+        <f>F4/G4</f>
+        <v>0.36279036248201296</v>
       </c>
       <c r="I4" s="2"/>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -667,11 +670,12 @@
         <v>906539</v>
       </c>
       <c r="H5" s="1">
-        <v>-0.63885502995458554</v>
+        <f>F5/G5</f>
+        <v>0.36114497004541446</v>
       </c>
       <c r="I5" s="2"/>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -694,11 +698,12 @@
         <v>985862</v>
       </c>
       <c r="H6" s="1">
-        <v>-0.6141305781133668</v>
+        <f>F6/G6</f>
+        <v>0.3858694218866332</v>
       </c>
       <c r="I6" s="2"/>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -721,11 +726,12 @@
         <v>1038128</v>
       </c>
       <c r="H7" s="1">
-        <v>-0.50022636900266626</v>
+        <f>F7/G7</f>
+        <v>0.49977363099733368</v>
       </c>
       <c r="I7" s="2"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -748,11 +754,12 @@
         <v>1092562</v>
       </c>
       <c r="H8" s="1">
-        <v>-0.34804798263164927</v>
+        <f>F8/G8</f>
+        <v>0.65195201736835073</v>
       </c>
       <c r="I8" s="2"/>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -775,11 +782,12 @@
         <v>1080554</v>
       </c>
       <c r="H9" s="1">
-        <v>-0.2937456156749223</v>
+        <f>F9/G9</f>
+        <v>0.7062543843250777</v>
       </c>
       <c r="I9" s="2"/>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -802,11 +810,12 @@
         <v>1034322</v>
       </c>
       <c r="H10" s="1">
-        <v>-0.29584597446443173</v>
+        <f>F10/G10</f>
+        <v>0.70415402553556827</v>
       </c>
       <c r="I10" s="2"/>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>9</v>
       </c>
@@ -829,11 +838,12 @@
         <v>980049</v>
       </c>
       <c r="H11" s="1">
-        <v>-0.26648565530907131</v>
+        <f>F11/G11</f>
+        <v>0.73351434469092869</v>
       </c>
       <c r="I11" s="2"/>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>10</v>
       </c>
@@ -856,11 +866,12 @@
         <v>801961</v>
       </c>
       <c r="H12" s="1">
-        <v>-0.22825798262010244</v>
+        <f>F12/G12</f>
+        <v>0.77174201737989756</v>
       </c>
       <c r="I12" s="2"/>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>11</v>
       </c>
@@ -883,11 +894,12 @@
         <v>793617</v>
       </c>
       <c r="H13" s="1">
-        <v>-0.21845802194257435</v>
+        <f>F13/G13</f>
+        <v>0.78154197805742565</v>
       </c>
       <c r="I13" s="2"/>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>20</v>
       </c>
@@ -910,87 +922,10 @@
         <v>11085302</v>
       </c>
       <c r="H14" s="1">
-        <v>-0.43792672495526053</v>
+        <f>F14/G14</f>
+        <v>0.56207327504473947</v>
       </c>
       <c r="I14" s="2"/>
-    </row>
-    <row r="17" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G17" s="1">
-        <f>F2/G2-1</f>
-        <v>-0.63768518977070565</v>
-      </c>
-    </row>
-    <row r="18" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G18" s="1">
-        <f>F3/G3-1</f>
-        <v>-0.66125435946232058</v>
-      </c>
-    </row>
-    <row r="19" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G19" s="1">
-        <f>F4/G4-1</f>
-        <v>-0.63720963751798698</v>
-      </c>
-    </row>
-    <row r="20" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G20" s="1">
-        <f>F5/G5-1</f>
-        <v>-0.63885502995458554</v>
-      </c>
-    </row>
-    <row r="21" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G21" s="1">
-        <f>F6/G6-1</f>
-        <v>-0.6141305781133668</v>
-      </c>
-    </row>
-    <row r="22" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G22" s="1">
-        <f>F7/G7-1</f>
-        <v>-0.50022636900266626</v>
-      </c>
-    </row>
-    <row r="23" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G23" s="1">
-        <f>F8/G8-1</f>
-        <v>-0.34804798263164927</v>
-      </c>
-    </row>
-    <row r="24" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G24" s="1">
-        <f>F9/G9-1</f>
-        <v>-0.2937456156749223</v>
-      </c>
-    </row>
-    <row r="25" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G25" s="1">
-        <f>F10/G10-1</f>
-        <v>-0.29584597446443173</v>
-      </c>
-    </row>
-    <row r="26" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G26" s="1">
-        <f>F11/G11-1</f>
-        <v>-0.26648565530907131</v>
-      </c>
-    </row>
-    <row r="27" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G27" s="1">
-        <f>F12/G12-1</f>
-        <v>-0.22825798262010244</v>
-      </c>
-    </row>
-    <row r="28" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G28" s="1">
-        <f>F13/G13-1</f>
-        <v>-0.21845802194257435</v>
-      </c>
-    </row>
-    <row r="29" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G29" s="1">
-        <f>F14/G14-1</f>
-        <v>-0.43792672495526053</v>
-      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -998,12 +933,9 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1230,15 +1162,19 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D5F8F857-E121-4686-AFAF-A3028DE7EF87}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{31941510-E3C3-4953-8B32-BA17BDE21C03}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -1263,10 +1199,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{31941510-E3C3-4953-8B32-BA17BDE21C03}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D5F8F857-E121-4686-AFAF-A3028DE7EF87}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>